<commit_message>
Added 1 more country to exluded
</commit_message>
<xml_diff>
--- a/excludedCountries.xlsx
+++ b/excludedCountries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\EECS4414\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEDBF620-EC00-4DB4-A075-4BAFA7D35E43}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B011C7-294F-4C15-A8A7-1D0ED9ED5815}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" xr2:uid="{1367362F-353F-40B5-A481-8B4A3830024D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>COD</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Serbia</t>
+  </si>
+  <si>
+    <t>TLS</t>
+  </si>
+  <si>
+    <t>Timor-Leste</t>
   </si>
 </sst>
 </file>
@@ -407,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A612B443-D9E1-4068-8B23-1A222AC8F8D6}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:D5"/>
+      <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,6 +491,20 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>-8.8742169999999998</v>
+      </c>
+      <c r="C6">
+        <v>125.72753899999999</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>